<commit_message>
New workflows added and Throw exceptions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -131,12 +131,18 @@
   <si>
     <t>FannieMae_LoginURL</t>
   </si>
+  <si>
+    <t>FMCredentials</t>
+  </si>
+  <si>
+    <t>FannieMae_LoginCredentials</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -166,6 +172,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -187,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -198,6 +210,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +528,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -583,7 +596,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2698,7 +2718,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Send mail added, Validation removed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\nsbotprod1\Desktop\Projects\uipath-investorstip-fanniemae\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\nsbotprod1\Desktop\Projects\wyndham-secondary-marketing-fanniemae\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -36,88 +36,6 @@
   </si>
   <si>
     <t>Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t>MaxRetryNumber</t>
-  </si>
-  <si>
-    <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
-    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionDataError</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
-    <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
-  </si>
-  <si>
-    <t>LogMessage_BusinessRuleException</t>
-  </si>
-  <si>
-    <t>Business rule exception.</t>
-  </si>
-  <si>
-    <t>LogMessage_ApplicationException</t>
-  </si>
-  <si>
-    <t>System exception.</t>
-  </si>
-  <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
   </si>
   <si>
     <t>SecondaryMarketing_SharedDrivePath</t>
@@ -136,6 +54,30 @@
   </si>
   <si>
     <t>FannieMae_LoginCredentials</t>
+  </si>
+  <si>
+    <t>SMTP - Server</t>
+  </si>
+  <si>
+    <t>SMTP - Port</t>
+  </si>
+  <si>
+    <t>SMTP - Credential</t>
+  </si>
+  <si>
+    <t>SmtpServer</t>
+  </si>
+  <si>
+    <t>SmtpPort</t>
+  </si>
+  <si>
+    <t>SmtpRecipient</t>
+  </si>
+  <si>
+    <t>SmtpCredentials</t>
+  </si>
+  <si>
+    <t>Smtp_Recipient</t>
   </si>
 </sst>
 </file>
@@ -199,14 +141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -525,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -575,35 +514,22 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
-      <c r="A4" t="s">
-        <v>20</v>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
+      <c r="B3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1593,9 +1519,6 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1607,7 +1530,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="A2:D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1651,85 +1576,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>26</v>
-      </c>
+    <row r="2" spans="1:26">
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2715,10 +2572,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1000"/>
+  <dimension ref="A1:Y999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2763,23 +2620,44 @@
     </row>
     <row r="2" spans="1:25" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:25" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:25" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="7" spans="1:25" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:25" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:25" ht="14.25" customHeight="1"/>
@@ -3773,7 +3651,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Download file bug fixed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>Smtp_Recipient</t>
+  </si>
+  <si>
+    <t>LoginRetry</t>
+  </si>
+  <si>
+    <t>FannieMae_LoginRetry</t>
+  </si>
+  <si>
+    <t>SetLoginRetry</t>
   </si>
 </sst>
 </file>
@@ -467,7 +476,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -528,7 +537,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2575,7 +2591,7 @@
   <dimension ref="A1:Y999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2658,7 +2674,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="8" spans="1:25" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:25" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:25" ht="14.25" customHeight="1"/>

</xml_diff>